<commit_message>
analyse des possibilités d'amelioration
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO (1).xlsx
+++ b/Modèle-audit-SEO (1).xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7490" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="7490" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="audit" sheetId="3" r:id="rId1"/>
-    <sheet name="analyse chiffrée" sheetId="4" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="5" r:id="rId2"/>
+    <sheet name="analyse chiffrée" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
   <si>
     <t>Catégorie</t>
   </si>
@@ -69,15 +70,9 @@
     <t>global code modifié (contact,html)</t>
   </si>
   <si>
-    <t>Supression de certaine resources js et css</t>
-  </si>
-  <si>
     <t>Suppression de css inutile</t>
   </si>
   <si>
-    <t>compression de js et css/bootstrap</t>
-  </si>
-  <si>
     <t>titres correctement ordonnés</t>
   </si>
   <si>
@@ -99,9 +94,6 @@
     <t>Balise Meta description, rajout de mots clés</t>
   </si>
   <si>
-    <t>Suppression de balise Meta keyword</t>
-  </si>
-  <si>
     <t>Suppression des keywords cachés</t>
   </si>
   <si>
@@ -114,33 +106,15 @@
     <t>contraste plus important,background/texte</t>
   </si>
   <si>
-    <t>des ressources inutiles ralentissent le chargement de la page</t>
-  </si>
-  <si>
     <t>css inutile ralentit le chargement de la page</t>
   </si>
   <si>
-    <t>inscrire les bonnes ressources</t>
-  </si>
-  <si>
-    <t>ressources js css inutiles</t>
-  </si>
-  <si>
     <t>css inutile dans certains blocs</t>
   </si>
   <si>
     <t>ecrire seulement le css nécessaire</t>
   </si>
   <si>
-    <t>les dossiers js et css-bootstrap trop long a charger</t>
-  </si>
-  <si>
-    <t>compresser ces dossiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dossiers trop importants </t>
-  </si>
-  <si>
     <t>compresser les images</t>
   </si>
   <si>
@@ -195,12 +169,6 @@
     <t>enregistre img 100% dans mediaquerry</t>
   </si>
   <si>
-    <t>Suppression de la balise keywords</t>
-  </si>
-  <si>
-    <t>en 2022 cla n'a plus d'intérêts</t>
-  </si>
-  <si>
     <t>ne pas mettre cette balise, mettre des keywords dans la balise description</t>
   </si>
   <si>
@@ -225,12 +193,6 @@
     <t>il faut être précis</t>
   </si>
   <si>
-    <t>balise footer inexistante</t>
-  </si>
-  <si>
-    <t>rajouter la balise footer</t>
-  </si>
-  <si>
     <t>la page web n'a pas de titre donc ralentissement de l'ouverture</t>
   </si>
   <si>
@@ -240,83 +202,113 @@
     <t>c'est la balise ou l'on peut afficher des mots clé dans une phrase de présentation</t>
   </si>
   <si>
-    <t>inutile en 2022</t>
-  </si>
-  <si>
-    <t>peu faire baisser le positionnement du site web</t>
-  </si>
-  <si>
     <t xml:space="preserve">correction de la langue, fr </t>
   </si>
   <si>
-    <t>corrigé le fait queça soit en anglais</t>
-  </si>
-  <si>
-    <t>MDN WEB DOCS</t>
-  </si>
-  <si>
-    <t>cour OC alleger les pages de votre site</t>
-  </si>
-  <si>
-    <t>compressor,io</t>
-  </si>
-  <si>
-    <t>compression de js et css/bootstrap minification</t>
-  </si>
-  <si>
-    <t>website planet</t>
-  </si>
-  <si>
     <t>google lighthouse</t>
   </si>
   <si>
-    <t>Grafikart</t>
-  </si>
-  <si>
-    <t>cours OC</t>
-  </si>
-  <si>
-    <t>Semrush Blog</t>
-  </si>
-  <si>
     <t xml:space="preserve">mettre fr </t>
   </si>
   <si>
-    <t>Rank info</t>
-  </si>
-  <si>
-    <t>Tutowebdesign</t>
-  </si>
-  <si>
-    <t>Mdn Webdocs</t>
-  </si>
-  <si>
-    <t>google n'apprecie pas le backlink</t>
-  </si>
-  <si>
     <t>mettre un lien dans la zone de contenu utile</t>
   </si>
   <si>
     <t>page annexe renommée, (contact)c'est clair pour lr robot google</t>
   </si>
   <si>
-    <t>comexplorer</t>
-  </si>
-  <si>
-    <t>anthedesign</t>
-  </si>
-  <si>
     <t>global code modifié (index,html)</t>
   </si>
   <si>
     <t>https://philippeeyraud.github.io/PhilippeEyraud_4_13012022/</t>
+  </si>
+  <si>
+    <t>h2 était ligne183</t>
+  </si>
+  <si>
+    <t>mettre h2 avant h3</t>
+  </si>
+  <si>
+    <t>corrigé le fait que cela soit en anglais</t>
+  </si>
+  <si>
+    <t>Jquery:2.10 est une version obsolète</t>
+  </si>
+  <si>
+    <t>version obsolete</t>
+  </si>
+  <si>
+    <t>version obsolete, metre en standby</t>
+  </si>
+  <si>
+    <t>ressources js css ralentissent la page</t>
+  </si>
+  <si>
+    <t>des ressources  ralentissent le chargement de la page</t>
+  </si>
+  <si>
+    <t>compression des images</t>
+  </si>
+  <si>
+    <t>en 2022 cela n'a plus d'intérêts</t>
+  </si>
+  <si>
+    <t>alleger les  ressources</t>
+  </si>
+  <si>
+    <t>minifier css js</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Glossary/minification</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/1603881-apprenez-a-creer-votre-site-web-avec-html5-et-css3/1608357-memento-des-balises-html</t>
+  </si>
+  <si>
+    <t>https://image.online-convert.com/fr/convertir-en-webp</t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/</t>
+  </si>
+  <si>
+    <t>https://compressor.io/</t>
+  </si>
+  <si>
+    <t>https://tutowebdesign.com/balise-title-html.php</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Learn/CSS/Styling_text/Fundamentals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=wu1Sk8iOPnE  Grafikart </t>
+  </si>
+  <si>
+    <t>https://www.webrankinfo.com/dossiers/debutants/meta-keywords</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578343-optimisez-le-contenu-de-vos-pages</t>
+  </si>
+  <si>
+    <t>https://blog.comexplorer.com/attribut-alt-images-interet</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Glossary/Tag</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-on-page-balise-meta-description/#:~:text=Les%203%20crit%C3%A8res%20primordiaux%20de,sinon%20Google%20va%20la%20couper.</t>
+  </si>
+  <si>
+    <t>Suppression de la balise Meta keywords</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,11 +342,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF24292F"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -519,9 +506,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,9 +569,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -594,12 +578,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -612,38 +590,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -784,7 +757,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>107949</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -899,6 +872,43 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="302185"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 3" descr="WebRankInfo"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17092706" y="2136588"/>
+          <a:ext cx="304800" cy="302185"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1203,20 +1213,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.69140625" customWidth="1"/>
-    <col min="2" max="2" width="50.15234375" customWidth="1"/>
-    <col min="3" max="3" width="27.15234375" customWidth="1"/>
-    <col min="4" max="4" width="24.23046875" customWidth="1"/>
-    <col min="5" max="5" width="33.3828125" customWidth="1"/>
-    <col min="6" max="6" width="18.23046875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="37.23046875" customWidth="1"/>
+    <col min="3" max="3" width="56.15234375" customWidth="1"/>
+    <col min="4" max="4" width="45.07421875" customWidth="1"/>
+    <col min="5" max="5" width="55.921875" customWidth="1"/>
+    <col min="6" max="6" width="128.07421875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="18" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1251,91 +1263,89 @@
         <v>6</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C3" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29"/>
-      <c r="B7" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>76</v>
+      <c r="E7" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1349,92 +1359,92 @@
       <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="30"/>
+      <c r="B10" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22"/>
+      <c r="B11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C12" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D12" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
-      <c r="B10" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="25" t="s">
+      <c r="F12" s="37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="D13" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="38" t="s">
-        <v>80</v>
+      <c r="F13" s="37" t="s">
+        <v>83</v>
       </c>
       <c r="G13" s="13"/>
     </row>
@@ -1450,75 +1460,75 @@
       <c r="A15" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="39" t="s">
+      <c r="B15" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="22"/>
+      <c r="B17" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="26" t="s">
+      <c r="D18" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="39" t="s">
         <v>85</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
-      <c r="B18" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1533,119 +1543,124 @@
       <c r="A20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22"/>
+      <c r="B21" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24" t="s">
+      <c r="C22" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="28" t="s">
+      <c r="C23" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="34"/>
+      <c r="B24" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>70</v>
-      </c>
       <c r="D24" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="44"/>
-      <c r="B25" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="E24" s="27"/>
+      <c r="F24" s="37" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F7" r:id="rId3"/>
+    <hyperlink ref="F11" r:id="rId4"/>
+    <hyperlink ref="F13" r:id="rId5"/>
+    <hyperlink ref="F15" r:id="rId6"/>
+    <hyperlink ref="F18" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1658,8 +1673,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>93</v>
+      <c r="A1" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="F1" s="11"/>
     </row>
@@ -1688,10 +1703,10 @@
         <v>52</v>
       </c>
       <c r="C3" s="2">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2">
         <v>78</v>
@@ -1702,7 +1717,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2">
         <v>82</v>
@@ -1716,13 +1731,13 @@
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>

</xml_diff>